<commit_message>
Working on DELETE. Rows are deleted properly, but the range isn't properly updated
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>State</t>
   </si>
@@ -187,7 +187,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts/>
+  <fonts x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills>
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,7 +205,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders>
     <border>
       <left/>
       <right/>
@@ -216,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -544,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C52"/>
+  <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>